<commit_message>
Unoptimized Solution report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/UnoptimizedSolution/power/UnoptimizedSolutionClockEnablePowerReport.xlsx
+++ b/reports/vivado/UnoptimizedSolution/power/UnoptimizedSolutionClockEnablePowerReport.xlsx
@@ -214,7 +214,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>4.6644549001939595E-4</v>
+        <v>4.542274691630155E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -240,16 +240,16 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>1.2618374603334814E-4</v>
+        <v>1.223599974764511E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>44.42307662963867</v>
+        <v>43.07692337036133</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>22.296903610229492</v>
+        <v>21.538461685180664</v>
       </c>
       <c r="E3" t="n" s="7">
         <v>74.0</v>
@@ -266,16 +266,16 @@
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>1.1141307913931087E-4</v>
+        <v>1.0876038868445903E-4</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>13</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>48.46154022216797</v>
+        <v>47.30769348144531</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>24.23076820373535</v>
+        <v>23.653844833374023</v>
       </c>
       <c r="E4" t="n" s="7">
         <v>105.0</v>
@@ -292,16 +292,16 @@
     </row>
     <row r="5" outlineLevel="1">
       <c r="A5" t="n" s="5">
-        <v>6.444202153943479E-5</v>
+        <v>6.291375029832125E-5</v>
       </c>
       <c r="B5" t="s" s="4">
         <v>15</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>48.653846740722656</v>
+        <v>47.5</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>43.238460540771484</v>
+        <v>41.98219299316406</v>
       </c>
       <c r="E5" t="n" s="7">
         <v>34.0</v>
@@ -318,16 +318,16 @@
     </row>
     <row r="6" outlineLevel="1">
       <c r="A6" t="n" s="5">
-        <v>3.996913437731564E-5</v>
+        <v>3.8863268855493516E-5</v>
       </c>
       <c r="B6" t="s" s="4">
         <v>17</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>48.653846740722656</v>
+        <v>47.30769348144531</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>24.387020111083984</v>
+        <v>23.653844833374023</v>
       </c>
       <c r="E6" t="n" s="7">
         <v>32.0</v>
@@ -344,16 +344,16 @@
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" t="n" s="5">
-        <v>3.9035770896589383E-5</v>
+        <v>3.810634734691121E-5</v>
       </c>
       <c r="B7" t="s" s="4">
         <v>19</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>48.46154022216797</v>
+        <v>47.30769348144531</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>24.23076820373535</v>
+        <v>23.653844833374023</v>
       </c>
       <c r="E7" t="n" s="7">
         <v>32.0</v>
@@ -370,16 +370,16 @@
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" t="n" s="5">
-        <v>3.1779807613929734E-5</v>
+        <v>3.0950770451454446E-5</v>
       </c>
       <c r="B8" t="s" s="4">
         <v>21</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>44.230770111083984</v>
+        <v>43.07692337036133</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>22.11538314819336</v>
+        <v>21.538461685180664</v>
       </c>
       <c r="E8" t="n" s="7">
         <v>20.0</v>
@@ -396,16 +396,16 @@
     </row>
     <row r="9" outlineLevel="1">
       <c r="A9" t="n" s="5">
-        <v>2.794499960145913E-5</v>
+        <v>2.7236250389250927E-5</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>22</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>53.07692337036133</v>
+        <v>51.730770111083984</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>26.538461685180664</v>
+        <v>25.94953727722168</v>
       </c>
       <c r="E9" t="n" s="7">
         <v>8.0</v>
@@ -422,16 +422,16 @@
     </row>
     <row r="10" outlineLevel="1">
       <c r="A10" t="n" s="5">
-        <v>1.62846154125873E-5</v>
+        <v>1.579326817591209E-5</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>24</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>44.61538314819336</v>
+        <v>43.269229888916016</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>22.30769157409668</v>
+        <v>21.698057174682617</v>
       </c>
       <c r="E10" t="n" s="7">
         <v>5.0</v>
@@ -448,16 +448,16 @@
     </row>
     <row r="11" outlineLevel="1">
       <c r="A11" t="n" s="5">
-        <v>6.2515387071471196E-6</v>
+        <v>6.102692623244366E-6</v>
       </c>
       <c r="B11" t="s" s="4">
         <v>25</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>48.46154022216797</v>
+        <v>47.30769348144531</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>23.95386505126953</v>
+        <v>23.376941680908203</v>
       </c>
       <c r="E11" t="n" s="7">
         <v>1.0</v>
@@ -483,7 +483,7 @@
         <v>4.615385055541992</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>2.178558111190796</v>
+        <v>2.274712085723877</v>
       </c>
       <c r="E12" t="n" s="7">
         <v>32.0</v>

</xml_diff>